<commit_message>
agg btn delete all, reload, verify input class
</commit_message>
<xml_diff>
--- a/private/uploads/upload.xlsx
+++ b/private/uploads/upload.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnonymousCsc\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B985B731-7817-49A6-950F-CB5B829D582F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE703621-1CBE-4DF0-A537-27C1074CE353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{015FB355-4E2D-41A8-B027-1FA3BBBE1324}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,105 +34,91 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>apellido</t>
-  </si>
-  <si>
-    <t>cedula</t>
-  </si>
-  <si>
-    <t>correo</t>
-  </si>
-  <si>
-    <t>contrasena</t>
-  </si>
-  <si>
-    <t>benito</t>
-  </si>
-  <si>
-    <t>camela</t>
-  </si>
-  <si>
-    <t>202365benito</t>
-  </si>
-  <si>
-    <t>maria</t>
-  </si>
-  <si>
-    <t>benito1@unicesar.edu.co</t>
-  </si>
-  <si>
-    <t>benito2@unicesar.edu.co</t>
-  </si>
-  <si>
-    <t>benito23@unicesar.edu.co</t>
-  </si>
-  <si>
-    <t>benito1111111@unicesar.edu.co</t>
-  </si>
-  <si>
-    <t>benitosdqe2@unicesar.edu.co</t>
-  </si>
-  <si>
-    <t>benito2ad1@unicesar.edu.co</t>
-  </si>
-  <si>
-    <t>juan 2</t>
-  </si>
-  <si>
-    <t>juan 3</t>
-  </si>
-  <si>
-    <t>juan 4</t>
-  </si>
-  <si>
-    <t>juan 5</t>
-  </si>
-  <si>
-    <t>maria2</t>
-  </si>
-  <si>
-    <t>maria3</t>
-  </si>
-  <si>
-    <t>maria4</t>
-  </si>
-  <si>
-    <t>maria5</t>
-  </si>
-  <si>
-    <t>juan</t>
+    <t>supervisor</t>
+  </si>
+  <si>
+    <t>docente</t>
+  </si>
+  <si>
+    <t>asignatura</t>
+  </si>
+  <si>
+    <t>dia</t>
+  </si>
+  <si>
+    <t>hora_inicio</t>
+  </si>
+  <si>
+    <t>hora_fin</t>
+  </si>
+  <si>
+    <t>salon</t>
+  </si>
+  <si>
+    <t>fecha_inicio</t>
+  </si>
+  <si>
+    <t>Calculo 2</t>
+  </si>
+  <si>
+    <t>Martes</t>
+  </si>
+  <si>
+    <t>fecha_fin</t>
+  </si>
+  <si>
+    <t>Programcion 2</t>
+  </si>
+  <si>
+    <t>Ingles</t>
+  </si>
+  <si>
+    <t>Jueves</t>
+  </si>
+  <si>
+    <t>Lunes</t>
+  </si>
+  <si>
+    <t>Algebra</t>
+  </si>
+  <si>
+    <t>Viernes</t>
+  </si>
+  <si>
+    <t>Sabado</t>
+  </si>
+  <si>
+    <t>Redes I</t>
+  </si>
+  <si>
+    <t>Redes II</t>
+  </si>
+  <si>
+    <t>Proyecto de grado I</t>
+  </si>
+  <si>
+    <t>Arquitectura de computadores</t>
+  </si>
+  <si>
+    <t>Miercoles</t>
+  </si>
+  <si>
+    <t>lab sistemas</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -165,19 +149,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -510,16 +491,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCAD9A26-B18F-4720-A080-BCFDDAD853DF}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="30" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -527,161 +512,329 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
+      <c r="B2">
+        <v>1212121212</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>10256325</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G2">
+        <v>112</v>
+      </c>
+      <c r="H2">
+        <v>1111111111</v>
+      </c>
+      <c r="I2" s="2">
+        <v>45746</v>
+      </c>
+      <c r="J2" s="2">
+        <v>45777</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1212121212</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3">
-        <v>1025632523</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="G3">
+        <v>105</v>
+      </c>
+      <c r="H3">
+        <v>1111111111</v>
+      </c>
+      <c r="I3" s="2">
+        <v>45747</v>
+      </c>
+      <c r="J3" s="2">
+        <v>45778</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1212121212</v>
+      </c>
+      <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4">
-        <v>1025633333</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>8</v>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="G4">
+        <v>201</v>
+      </c>
+      <c r="H4">
+        <v>1111111111</v>
+      </c>
+      <c r="I4" s="2">
+        <v>45748</v>
+      </c>
+      <c r="J4" s="2">
+        <v>45779</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1212121212</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5">
-        <v>1088888823</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>8</v>
+      <c r="E5" s="1">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.55208333333333337</v>
+      </c>
+      <c r="G5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5">
+        <v>78787878</v>
+      </c>
+      <c r="I5" s="2">
+        <v>45749</v>
+      </c>
+      <c r="J5" s="2">
+        <v>45780</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>15</v>
-      </c>
-      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>33333333333</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
         <v>18</v>
       </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6">
-        <v>1025999993</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>8</v>
+      <c r="E6" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="G6">
+        <v>105</v>
+      </c>
+      <c r="H6">
+        <v>78787878</v>
+      </c>
+      <c r="I6" s="2">
+        <v>45750</v>
+      </c>
+      <c r="J6" s="2">
+        <v>45781</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>19191919</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="G7">
+        <v>102</v>
+      </c>
+      <c r="H7">
+        <v>78787878</v>
+      </c>
+      <c r="I7" s="2">
+        <v>45751</v>
+      </c>
+      <c r="J7" s="2">
+        <v>45782</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>19191919</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.25</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G8">
+        <v>202</v>
+      </c>
+      <c r="H8">
+        <v>33737334</v>
+      </c>
+      <c r="I8" s="2">
+        <v>45752</v>
+      </c>
+      <c r="J8" s="2">
+        <v>45783</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2323233444</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="G9">
+        <v>114</v>
+      </c>
+      <c r="H9">
+        <v>33737334</v>
+      </c>
+      <c r="I9" s="2">
+        <v>45753</v>
+      </c>
+      <c r="J9" s="2">
+        <v>45784</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>2323233444</v>
+      </c>
+      <c r="C10" t="s">
         <v>16</v>
       </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7">
-        <v>1022221113</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I8" s="4"/>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="G10">
+        <v>500</v>
+      </c>
+      <c r="H10">
+        <v>32541215</v>
+      </c>
+      <c r="I10" s="2">
+        <v>45754</v>
+      </c>
+      <c r="J10" s="2">
+        <v>45785</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="E12" s="4"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="I16" s="3"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{42A18433-1351-4FF3-9874-CCD1CB667423}"/>
-    <hyperlink ref="E3:E7" r:id="rId2" display="benito@unicesar.edu.co" xr:uid="{EF4BBFCA-21E4-4BA6-9688-0D57637CC136}"/>
-    <hyperlink ref="E3" r:id="rId3" xr:uid="{D411F6F8-97AC-41E9-8D42-BD912DD79C4B}"/>
-    <hyperlink ref="E4" r:id="rId4" xr:uid="{2EA4DA9D-B51B-414B-B772-248614C075B3}"/>
-    <hyperlink ref="E5" r:id="rId5" xr:uid="{89D3AAB6-580F-4919-8DBB-AE24A60235B2}"/>
-    <hyperlink ref="E6" r:id="rId6" xr:uid="{80BD506C-ABCF-48BC-92B5-99CEC9D0350F}"/>
-    <hyperlink ref="E7" r:id="rId7" xr:uid="{7875FAA3-C79E-4529-AE6E-72F28505FB1A}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes btn del all teacher, supervis
</commit_message>
<xml_diff>
--- a/private/uploads/upload.xlsx
+++ b/private/uploads/upload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnonymousCsc\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE703621-1CBE-4DF0-A537-27C1074CE353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B480B8-7B62-47DF-BBAD-98CE626D7AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{015FB355-4E2D-41A8-B027-1FA3BBBE1324}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{015FB355-4E2D-41A8-B027-1FA3BBBE1324}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,81 +34,132 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>supervisor</t>
-  </si>
-  <si>
-    <t>docente</t>
-  </si>
-  <si>
-    <t>asignatura</t>
-  </si>
-  <si>
-    <t>dia</t>
-  </si>
-  <si>
-    <t>hora_inicio</t>
-  </si>
-  <si>
-    <t>hora_fin</t>
-  </si>
-  <si>
-    <t>salon</t>
-  </si>
-  <si>
-    <t>fecha_inicio</t>
-  </si>
-  <si>
-    <t>Calculo 2</t>
-  </si>
-  <si>
-    <t>Martes</t>
-  </si>
-  <si>
-    <t>fecha_fin</t>
-  </si>
-  <si>
-    <t>Programcion 2</t>
-  </si>
-  <si>
-    <t>Ingles</t>
-  </si>
-  <si>
-    <t>Jueves</t>
-  </si>
-  <si>
-    <t>Lunes</t>
-  </si>
-  <si>
-    <t>Algebra</t>
-  </si>
-  <si>
-    <t>Viernes</t>
-  </si>
-  <si>
-    <t>Sabado</t>
-  </si>
-  <si>
-    <t>Redes I</t>
-  </si>
-  <si>
-    <t>Redes II</t>
-  </si>
-  <si>
-    <t>Proyecto de grado I</t>
-  </si>
-  <si>
-    <t>Arquitectura de computadores</t>
-  </si>
-  <si>
-    <t>Miercoles</t>
-  </si>
-  <si>
-    <t>lab sistemas</t>
+    <t>nombre</t>
+  </si>
+  <si>
+    <t>apellido</t>
+  </si>
+  <si>
+    <t>cedula</t>
+  </si>
+  <si>
+    <t>correo</t>
+  </si>
+  <si>
+    <t>contrasena</t>
+  </si>
+  <si>
+    <t>benito@unicesar.edu.co</t>
+  </si>
+  <si>
+    <t>202365benito</t>
+  </si>
+  <si>
+    <t>reyes</t>
+  </si>
+  <si>
+    <t>brenda</t>
+  </si>
+  <si>
+    <t>brenda@unicesar.edu.co</t>
+  </si>
+  <si>
+    <t>2025A@bren</t>
+  </si>
+  <si>
+    <t>juan</t>
+  </si>
+  <si>
+    <t>toro</t>
+  </si>
+  <si>
+    <t>juantoro@gmail.com</t>
+  </si>
+  <si>
+    <t>juan2025@A7</t>
+  </si>
+  <si>
+    <t>ana</t>
+  </si>
+  <si>
+    <t>lopez</t>
+  </si>
+  <si>
+    <t>analopez@gmail.com</t>
+  </si>
+  <si>
+    <t>marcos</t>
+  </si>
+  <si>
+    <t>marta</t>
+  </si>
+  <si>
+    <t>fernando</t>
+  </si>
+  <si>
+    <t>cristian</t>
+  </si>
+  <si>
+    <t>francisco</t>
+  </si>
+  <si>
+    <t>suarez</t>
+  </si>
+  <si>
+    <t>costa</t>
+  </si>
+  <si>
+    <t>plata</t>
+  </si>
+  <si>
+    <t>narvaez</t>
+  </si>
+  <si>
+    <t>coronel</t>
+  </si>
+  <si>
+    <t>marcos@gmail.com</t>
+  </si>
+  <si>
+    <t>marta@gmail.com</t>
+  </si>
+  <si>
+    <t>cristian@gmail.com</t>
+  </si>
+  <si>
+    <t>ferplata@gmail.com</t>
+  </si>
+  <si>
+    <t>anaA@120</t>
+  </si>
+  <si>
+    <t>Mar45aA@</t>
+  </si>
+  <si>
+    <t>452Marta@</t>
+  </si>
+  <si>
+    <t>fErna12A@</t>
+  </si>
+  <si>
+    <t>fran12@gmail.com</t>
+  </si>
+  <si>
+    <t>franA@14</t>
+  </si>
+  <si>
+    <t>487Snarva@</t>
+  </si>
+  <si>
+    <t>londona</t>
+  </si>
+  <si>
+    <t>silvia</t>
   </si>
 </sst>
 </file>
@@ -126,7 +177,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -149,16 +200,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -491,20 +545,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCAD9A26-B18F-4720-A080-BCFDDAD853DF}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -512,329 +563,215 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>5</v>
-      </c>
-      <c r="F1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
-        <v>1212121212</v>
+      <c r="B2" t="s">
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="F2" s="1">
-        <v>0.58333333333333337</v>
-      </c>
-      <c r="G2">
-        <v>112</v>
-      </c>
-      <c r="H2">
-        <v>1111111111</v>
-      </c>
-      <c r="I2" s="2">
-        <v>45746</v>
-      </c>
-      <c r="J2" s="2">
-        <v>45777</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="D2">
+        <v>10256325</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>1212121212</v>
+      <c r="B3" t="s">
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="G3">
-        <v>105</v>
-      </c>
-      <c r="H3">
-        <v>1111111111</v>
-      </c>
-      <c r="I3" s="2">
-        <v>45747</v>
-      </c>
-      <c r="J3" s="2">
-        <v>45778</v>
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>49578785</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>1212121212</v>
+      <c r="B4" t="s">
+        <v>12</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4">
+        <v>45896123</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
         <v>15</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.375</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="G4">
-        <v>201</v>
-      </c>
-      <c r="H4">
-        <v>1111111111</v>
-      </c>
-      <c r="I4" s="2">
-        <v>45748</v>
-      </c>
-      <c r="J4" s="2">
-        <v>45779</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5">
-        <v>1212121212</v>
+      <c r="B5" t="s">
+        <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="1">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="F5" s="1">
-        <v>0.55208333333333337</v>
-      </c>
-      <c r="G5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H5">
-        <v>78787878</v>
-      </c>
-      <c r="I5" s="2">
-        <v>45749</v>
-      </c>
-      <c r="J5" s="2">
-        <v>45780</v>
+      <c r="D5">
+        <v>45412454</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>33333333333</v>
+      <c r="B6" t="s">
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0.375</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="G6">
-        <v>105</v>
-      </c>
-      <c r="H6">
-        <v>78787878</v>
-      </c>
-      <c r="I6" s="2">
-        <v>45750</v>
-      </c>
-      <c r="J6" s="2">
-        <v>45781</v>
+        <v>24</v>
+      </c>
+      <c r="D6">
+        <v>45871267</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7">
-        <v>19191919</v>
+      <c r="B7" t="s">
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="G7">
-        <v>102</v>
-      </c>
-      <c r="H7">
-        <v>78787878</v>
-      </c>
-      <c r="I7" s="2">
-        <v>45751</v>
-      </c>
-      <c r="J7" s="2">
-        <v>45782</v>
+        <v>25</v>
+      </c>
+      <c r="D7">
+        <v>12012545</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8">
-        <v>19191919</v>
+      <c r="B8" t="s">
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0.25</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="G8">
-        <v>202</v>
-      </c>
-      <c r="H8">
-        <v>33737334</v>
-      </c>
-      <c r="I8" s="2">
-        <v>45752</v>
-      </c>
-      <c r="J8" s="2">
-        <v>45783</v>
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <v>45216325</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>2323233444</v>
+      <c r="B9" t="s">
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0.54166666666666663</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0.625</v>
-      </c>
-      <c r="G9">
-        <v>114</v>
-      </c>
-      <c r="H9">
-        <v>33737334</v>
-      </c>
-      <c r="I9" s="2">
-        <v>45753</v>
-      </c>
-      <c r="J9" s="2">
-        <v>45784</v>
+        <v>27</v>
+      </c>
+      <c r="D9">
+        <v>785413236</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>2323233444</v>
+      <c r="B10" t="s">
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="G10">
-        <v>500</v>
-      </c>
-      <c r="H10">
-        <v>32541215</v>
-      </c>
-      <c r="I10" s="2">
-        <v>45754</v>
-      </c>
-      <c r="J10" s="2">
-        <v>45785</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="G12" s="3"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I16" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="D10">
+        <v>14578733</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{42A18433-1351-4FF3-9874-CCD1CB667423}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{3E112FEE-1EB4-4E27-86F7-5E4564C51908}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{5A3E047B-E266-4100-B30A-CB541BCF7724}"/>
+    <hyperlink ref="E5" r:id="rId4" xr:uid="{22ECA433-C1EE-45C4-B2A6-8CB9D6C67CF1}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{2F3D6284-EAAF-467E-B4A6-ED03B530F3F5}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{293A6770-9C0A-4ACF-8444-6F088ED0D4BA}"/>
+    <hyperlink ref="E8" r:id="rId7" xr:uid="{9F1E4357-DD56-410C-B5BE-A00E7FA1AF07}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{263E14D8-AB00-4CE2-8F0F-4449179C9BEE}"/>
+    <hyperlink ref="E10" r:id="rId9" xr:uid="{079B5CA6-0BA6-4281-8BB0-2B31C67A5ADD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
horario endpoint consume fixed
</commit_message>
<xml_diff>
--- a/private/uploads/upload.xlsx
+++ b/private/uploads/upload.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnonymousCsc\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jerso\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B480B8-7B62-47DF-BBAD-98CE626D7AE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331662D9-5743-48A7-BC20-0AF945565FF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{015FB355-4E2D-41A8-B027-1FA3BBBE1324}"/>
+    <workbookView xWindow="12735" yWindow="1560" windowWidth="15585" windowHeight="11295" xr2:uid="{015FB355-4E2D-41A8-B027-1FA3BBBE1324}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,139 +36,94 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="27">
   <si>
     <t>id</t>
   </si>
   <si>
-    <t>nombre</t>
-  </si>
-  <si>
-    <t>apellido</t>
-  </si>
-  <si>
-    <t>cedula</t>
-  </si>
-  <si>
-    <t>correo</t>
-  </si>
-  <si>
-    <t>contrasena</t>
-  </si>
-  <si>
-    <t>benito@unicesar.edu.co</t>
-  </si>
-  <si>
-    <t>202365benito</t>
-  </si>
-  <si>
-    <t>reyes</t>
-  </si>
-  <si>
-    <t>brenda</t>
-  </si>
-  <si>
-    <t>brenda@unicesar.edu.co</t>
-  </si>
-  <si>
-    <t>2025A@bren</t>
-  </si>
-  <si>
-    <t>juan</t>
-  </si>
-  <si>
-    <t>toro</t>
-  </si>
-  <si>
-    <t>juantoro@gmail.com</t>
-  </si>
-  <si>
-    <t>juan2025@A7</t>
-  </si>
-  <si>
-    <t>ana</t>
-  </si>
-  <si>
-    <t>lopez</t>
-  </si>
-  <si>
-    <t>analopez@gmail.com</t>
-  </si>
-  <si>
-    <t>marcos</t>
-  </si>
-  <si>
-    <t>marta</t>
-  </si>
-  <si>
-    <t>fernando</t>
-  </si>
-  <si>
-    <t>cristian</t>
-  </si>
-  <si>
-    <t>francisco</t>
-  </si>
-  <si>
-    <t>suarez</t>
-  </si>
-  <si>
-    <t>costa</t>
-  </si>
-  <si>
-    <t>plata</t>
-  </si>
-  <si>
-    <t>narvaez</t>
-  </si>
-  <si>
-    <t>coronel</t>
-  </si>
-  <si>
-    <t>marcos@gmail.com</t>
-  </si>
-  <si>
-    <t>marta@gmail.com</t>
-  </si>
-  <si>
-    <t>cristian@gmail.com</t>
-  </si>
-  <si>
-    <t>ferplata@gmail.com</t>
-  </si>
-  <si>
-    <t>anaA@120</t>
-  </si>
-  <si>
-    <t>Mar45aA@</t>
-  </si>
-  <si>
-    <t>452Marta@</t>
-  </si>
-  <si>
-    <t>fErna12A@</t>
-  </si>
-  <si>
-    <t>fran12@gmail.com</t>
-  </si>
-  <si>
-    <t>franA@14</t>
-  </si>
-  <si>
-    <t>487Snarva@</t>
-  </si>
-  <si>
-    <t>londona</t>
-  </si>
-  <si>
-    <t>silvia</t>
+    <t>supervisor</t>
+  </si>
+  <si>
+    <t>docente</t>
+  </si>
+  <si>
+    <t>asignatura</t>
+  </si>
+  <si>
+    <t>dia</t>
+  </si>
+  <si>
+    <t>hora_inicio</t>
+  </si>
+  <si>
+    <t>hora_fin</t>
+  </si>
+  <si>
+    <t>salon</t>
+  </si>
+  <si>
+    <t>fecha_inicio</t>
+  </si>
+  <si>
+    <t>Calculo 2</t>
+  </si>
+  <si>
+    <t>Martes</t>
+  </si>
+  <si>
+    <t>fecha_fin</t>
+  </si>
+  <si>
+    <t>Calculo 3</t>
+  </si>
+  <si>
+    <t>Calculo 4</t>
+  </si>
+  <si>
+    <t>Calculo 5</t>
+  </si>
+  <si>
+    <t>Calculo 6</t>
+  </si>
+  <si>
+    <t>Calculo 7</t>
+  </si>
+  <si>
+    <t>Calculo 8</t>
+  </si>
+  <si>
+    <t>Calculo 9</t>
+  </si>
+  <si>
+    <t>Calculo 10</t>
+  </si>
+  <si>
+    <t>Calculo 11</t>
+  </si>
+  <si>
+    <t>Miércoles</t>
+  </si>
+  <si>
+    <t>Jueves</t>
+  </si>
+  <si>
+    <t>Viernes</t>
+  </si>
+  <si>
+    <t>Sábado</t>
+  </si>
+  <si>
+    <t>Domingo</t>
+  </si>
+  <si>
+    <t>Lunes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,9 +132,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,19 +163,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -545,17 +505,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCAD9A26-B18F-4720-A080-BCFDDAD853DF}">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -563,215 +521,363 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>41</v>
+      <c r="B2">
+        <v>32145214</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D2">
-        <v>10256325</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="G2">
+        <v>112</v>
+      </c>
+      <c r="H2">
+        <v>1005000001</v>
+      </c>
+      <c r="I2" s="2">
+        <v>45746</v>
+      </c>
+      <c r="J2" s="2">
+        <v>45777</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
+      <c r="B3">
+        <v>32145214</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>49578785</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="G3">
+        <v>112</v>
+      </c>
+      <c r="H3">
+        <v>1005000001</v>
+      </c>
+      <c r="I3" s="2">
+        <v>45747</v>
+      </c>
+      <c r="J3" s="2">
+        <v>45778</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
+      <c r="B4">
+        <v>32145214</v>
       </c>
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4">
-        <v>45896123</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.41666666666666702</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="G4">
+        <v>112</v>
+      </c>
+      <c r="H4">
+        <v>1005000001</v>
+      </c>
+      <c r="I4" s="2">
+        <v>45748</v>
+      </c>
+      <c r="J4" s="2">
+        <v>45779</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>16</v>
+      <c r="B5">
+        <v>32145214</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5">
-        <v>45412454</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" t="s">
-        <v>33</v>
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.45833333333333298</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="G5">
+        <v>112</v>
+      </c>
+      <c r="H5">
+        <v>1005000001</v>
+      </c>
+      <c r="I5" s="2">
+        <v>45749</v>
+      </c>
+      <c r="J5" s="2">
+        <v>45780</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>19</v>
+      <c r="B6">
+        <v>25489652</v>
       </c>
       <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
         <v>24</v>
       </c>
-      <c r="D6">
-        <v>45871267</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" t="s">
-        <v>34</v>
+      <c r="E6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="G6">
+        <v>112</v>
+      </c>
+      <c r="H6">
+        <v>1005000001</v>
+      </c>
+      <c r="I6" s="2">
+        <v>45750</v>
+      </c>
+      <c r="J6" s="2">
+        <v>45781</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>20</v>
+      <c r="B7">
+        <v>25489652</v>
       </c>
       <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
         <v>25</v>
       </c>
-      <c r="D7">
-        <v>12012545</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" t="s">
-        <v>35</v>
+      <c r="E7" s="1">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.79166666666666696</v>
+      </c>
+      <c r="G7">
+        <v>112</v>
+      </c>
+      <c r="H7">
+        <v>1005000001</v>
+      </c>
+      <c r="I7" s="2">
+        <v>45751</v>
+      </c>
+      <c r="J7" s="2">
+        <v>45782</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" t="s">
-        <v>21</v>
+      <c r="B8">
+        <v>25489652</v>
       </c>
       <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
         <v>26</v>
       </c>
-      <c r="D8">
-        <v>45216325</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" t="s">
-        <v>36</v>
+      <c r="E8" s="1">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.83333333333333304</v>
+      </c>
+      <c r="G8">
+        <v>112</v>
+      </c>
+      <c r="H8">
+        <v>1005000001</v>
+      </c>
+      <c r="I8" s="2">
+        <v>45752</v>
+      </c>
+      <c r="J8" s="2">
+        <v>45783</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
-        <v>22</v>
+      <c r="B9">
+        <v>22255544</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9">
-        <v>785413236</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" t="s">
-        <v>39</v>
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.625</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.875</v>
+      </c>
+      <c r="G9">
+        <v>112</v>
+      </c>
+      <c r="H9">
+        <v>1005000001</v>
+      </c>
+      <c r="I9" s="2">
+        <v>45753</v>
+      </c>
+      <c r="J9" s="2">
+        <v>45784</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
-        <v>23</v>
+      <c r="B10">
+        <v>22255544</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10">
-        <v>14578733</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" t="s">
-        <v>38</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.66666666666666696</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.91666666666666696</v>
+      </c>
+      <c r="G10">
+        <v>112</v>
+      </c>
+      <c r="H10">
+        <v>1005000001</v>
+      </c>
+      <c r="I10" s="2">
+        <v>45754</v>
+      </c>
+      <c r="J10" s="2">
+        <v>45785</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>22255544</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.95833333333333304</v>
+      </c>
+      <c r="G11">
+        <v>112</v>
+      </c>
+      <c r="H11">
+        <v>1005000001</v>
+      </c>
+      <c r="I11" s="2">
+        <v>45755</v>
+      </c>
+      <c r="J11" s="2">
+        <v>45786</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="F15" s="3"/>
+    </row>
+    <row r="17" spans="5:9" x14ac:dyDescent="0.25">
+      <c r="E17" s="3"/>
+      <c r="I17" s="3"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{42A18433-1351-4FF3-9874-CCD1CB667423}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{3E112FEE-1EB4-4E27-86F7-5E4564C51908}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{5A3E047B-E266-4100-B30A-CB541BCF7724}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{22ECA433-C1EE-45C4-B2A6-8CB9D6C67CF1}"/>
-    <hyperlink ref="E6" r:id="rId5" xr:uid="{2F3D6284-EAAF-467E-B4A6-ED03B530F3F5}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{293A6770-9C0A-4ACF-8444-6F088ED0D4BA}"/>
-    <hyperlink ref="E8" r:id="rId7" xr:uid="{9F1E4357-DD56-410C-B5BE-A00E7FA1AF07}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{263E14D8-AB00-4CE2-8F0F-4449179C9BEE}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{079B5CA6-0BA6-4281-8BB0-2B31C67A5ADD}"/>
-  </hyperlinks>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>